<commit_message>
updates figs and demos
</commit_message>
<xml_diff>
--- a/demos/Overview_demos.xlsx
+++ b/demos/Overview_demos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suzan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\Documents\GitHub\SdF\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC13126-8FEC-42B5-822B-4B47E3FA91DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B769F50-780B-4363-8EF2-7662C757902A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54D9BEBC-F946-48D8-A401-495DD07D3BFF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{54D9BEBC-F946-48D8-A401-495DD07D3BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="84">
   <si>
     <t>Demo number</t>
   </si>
@@ -214,6 +214,69 @@
   </si>
   <si>
     <t>Dutch text in figure</t>
+  </si>
+  <si>
+    <t>1 01</t>
+  </si>
+  <si>
+    <t>Opwaartse en Neerwaartsekracht</t>
+  </si>
+  <si>
+    <t>1 03</t>
+  </si>
+  <si>
+    <t>Waardoor stijgt het water?</t>
+  </si>
+  <si>
+    <t>1 10</t>
+  </si>
+  <si>
+    <t>Warm &amp; Koud, Zoet &amp; Zout</t>
+  </si>
+  <si>
+    <t>1 17</t>
+  </si>
+  <si>
+    <t>Blussen zonder water</t>
+  </si>
+  <si>
+    <t>1 21</t>
+  </si>
+  <si>
+    <t>Lucht is niet niks</t>
+  </si>
+  <si>
+    <t>1 29</t>
+  </si>
+  <si>
+    <t>Gloeilamp uitblazen</t>
+  </si>
+  <si>
+    <t>1 37</t>
+  </si>
+  <si>
+    <t>Twee veren, serie of parallel?</t>
+  </si>
+  <si>
+    <t>Schaduw van een vlam</t>
+  </si>
+  <si>
+    <t>1 52</t>
+  </si>
+  <si>
+    <t>1 57</t>
+  </si>
+  <si>
+    <t>Spelen met dichtheid</t>
+  </si>
+  <si>
+    <t>Vallend kaars</t>
+  </si>
+  <si>
+    <t>1 59</t>
+  </si>
+  <si>
+    <t>NL</t>
   </si>
 </sst>
 </file>
@@ -251,12 +314,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,10 +341,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -591,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D0A0FA-7B3B-48FB-A231-8EB90CFB0395}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,7 +1034,7 @@
       <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E20" t="s">
@@ -1001,7 +1071,7 @@
       <c r="C22" t="s">
         <v>24</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E22" t="s">
@@ -1038,7 +1108,7 @@
       <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E24" t="s">
@@ -1058,7 +1128,7 @@
       <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E25" t="s">
@@ -1078,7 +1148,7 @@
       <c r="C26" t="s">
         <v>28</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E26" t="s">
@@ -1086,6 +1156,466 @@
       </c>
       <c r="F26" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new demos and figs
</commit_message>
<xml_diff>
--- a/demos/Overview_demos.xlsx
+++ b/demos/Overview_demos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\Documents\GitHub\SdF\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A0CC60-3066-4A61-A470-4E928E52BB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769389A7-147B-4369-A930-05E955DEF3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1331,16 +1331,16 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21">
+      <c r="B21" s="4">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="4">
         <v>43</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F21" t="s">
@@ -1380,19 +1380,19 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23">
+      <c r="B23" s="4">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="4">
         <v>48</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F23" t="s">

</xml_diff>

<commit_message>
try to incl python
</commit_message>
<xml_diff>
--- a/demos/Overview_demos.xlsx
+++ b/demos/Overview_demos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\Documents\GitHub\SdF\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E482E23-D428-4020-8EE5-DB7EE7910DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B9522F-9881-41A1-A6A2-35D05076BABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="127">
   <si>
     <t>Demo name</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>Freek</t>
+  </si>
+  <si>
+    <t>Videotje toevoegen</t>
   </si>
 </sst>
 </file>
@@ -822,7 +825,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G87" sqref="G87"/>
+      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2752,6 +2755,9 @@
       <c r="E99" t="s">
         <v>116</v>
       </c>
+      <c r="F99" t="s">
+        <v>126</v>
+      </c>
       <c r="I99" t="s">
         <v>125</v>
       </c>

</xml_diff>